<commit_message>
Added support for ignoring off tasks
</commit_message>
<xml_diff>
--- a/tests/test_protocol_two_tasks.xlsx
+++ b/tests/test_protocol_two_tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A82C21-CE58-4F4D-A6A5-8EA7540E13DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55325B41-C06C-854D-B02C-ED2721E0A557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Pump</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>F.0.1.22_2</t>
+  </si>
+  <si>
+    <t>Dose multiplier interval</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:M3"/>
+      <selection activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,12 +564,14 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
@@ -611,12 +616,14 @@
         <v>6.8</v>
       </c>
       <c r="G2" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="13">
         <v>50</v>
       </c>
-      <c r="H2" s="13">
+      <c r="I2" s="13">
         <v>2</v>
       </c>
-      <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -661,12 +668,14 @@
         <v>6.8</v>
       </c>
       <c r="G3" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="13">
         <v>10</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="13">
         <v>2</v>
       </c>
-      <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>

</xml_diff>